<commit_message>
Add new sheet "june 2018"
</commit_message>
<xml_diff>
--- a/Monthly Statement.xlsx
+++ b/Monthly Statement.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760"/>
@@ -9,12 +9,13 @@
   <sheets>
     <sheet name="Revenue" sheetId="3" r:id="rId1"/>
     <sheet name="OPERATIONS" sheetId="4" r:id="rId2"/>
-    <sheet name="May 2018" sheetId="2" r:id="rId3"/>
+    <sheet name="June 2018" sheetId="5" r:id="rId3"/>
+    <sheet name="May 2018" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OPERATIONS!$B$3:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="192">
   <si>
     <t>Closed Trade P/L:</t>
   </si>
@@ -354,10 +355,6 @@
     <phoneticPr fontId="9"/>
   </si>
   <si>
-    <t>Rate/Month(%)</t>
-    <phoneticPr fontId="9"/>
-  </si>
-  <si>
     <t>Target</t>
     <phoneticPr fontId="9"/>
   </si>
@@ -368,6 +365,249 @@
   <si>
     <t>Status</t>
     <phoneticPr fontId="9"/>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t> 2018.06.15 20:29:27</t>
+  </si>
+  <si>
+    <t>Archived orders</t>
+  </si>
+  <si>
+    <t>1 753.12</t>
+  </si>
+  <si>
+    <t> 2018.05.23 07:40:42</t>
+  </si>
+  <si>
+    <t> 2018.06.13 06:26:35</t>
+  </si>
+  <si>
+    <t> 2018.05.23 13:36:26</t>
+  </si>
+  <si>
+    <t> 2018.06.27 02:39:26</t>
+  </si>
+  <si>
+    <t> 2018.05.29 06:14:16</t>
+  </si>
+  <si>
+    <t>eurcadm</t>
+  </si>
+  <si>
+    <t> 2018.06.01 18:10:00</t>
+  </si>
+  <si>
+    <t> 2018.06.04 12:47:29</t>
+  </si>
+  <si>
+    <t>nzdusdm</t>
+  </si>
+  <si>
+    <t> 2018.06.05 15:22:47</t>
+  </si>
+  <si>
+    <t> 2018.06.05 12:32:12</t>
+  </si>
+  <si>
+    <t>W-ZOTAVND-VND-60859180</t>
+  </si>
+  <si>
+    <t> 2018.06.05 15:27:52</t>
+  </si>
+  <si>
+    <t>eurnzdm</t>
+  </si>
+  <si>
+    <t> 2018.06.07 13:30:32</t>
+  </si>
+  <si>
+    <t> 2018.06.08 06:12:02</t>
+  </si>
+  <si>
+    <t> 2018.06.08 08:24:42</t>
+  </si>
+  <si>
+    <t> 2018.06.11 01:37:32</t>
+  </si>
+  <si>
+    <t>W-CC-USD-61123802</t>
+  </si>
+  <si>
+    <t> 2018.06.11 05:31:34</t>
+  </si>
+  <si>
+    <t> 2018.06.15 07:32:37</t>
+  </si>
+  <si>
+    <t> 2018.06.11 06:32:54</t>
+  </si>
+  <si>
+    <t> 2018.06.15 11:40:28</t>
+  </si>
+  <si>
+    <t> 2018.06.13 12:22:26</t>
+  </si>
+  <si>
+    <t> 2018.06.14 00:01:52</t>
+  </si>
+  <si>
+    <t> 2018.06.14 07:01:23</t>
+  </si>
+  <si>
+    <t> 2018.06.14 09:16:09</t>
+  </si>
+  <si>
+    <t> 2018.06.14 09:13:20</t>
+  </si>
+  <si>
+    <t>chfjpym</t>
+  </si>
+  <si>
+    <t> 2018.06.14 14:16:02</t>
+  </si>
+  <si>
+    <t> 2018.06.15 11:39:59</t>
+  </si>
+  <si>
+    <t> 2018.06.15 12:50:16</t>
+  </si>
+  <si>
+    <t> 2018.06.15 11:40:51</t>
+  </si>
+  <si>
+    <t> 2018.06.15 13:18:53</t>
+  </si>
+  <si>
+    <t> 2018.06.15 12:55:17</t>
+  </si>
+  <si>
+    <t> 2018.06.15 14:31:26</t>
+  </si>
+  <si>
+    <t> 2018.06.18 05:26:54</t>
+  </si>
+  <si>
+    <t> 2018.06.19 07:07:18</t>
+  </si>
+  <si>
+    <t> 2018.06.19 04:24:42</t>
+  </si>
+  <si>
+    <t>gbpaudm</t>
+  </si>
+  <si>
+    <t> 2018.06.19 06:59:59</t>
+  </si>
+  <si>
+    <t> 2018.06.19 07:00:11</t>
+  </si>
+  <si>
+    <t> 2018.06.19 10:46:10</t>
+  </si>
+  <si>
+    <t> 2018.06.19 07:40:58</t>
+  </si>
+  <si>
+    <t> 2018.06.19 10:45:55</t>
+  </si>
+  <si>
+    <t> 2018.06.19 10:46:31</t>
+  </si>
+  <si>
+    <t> 2018.06.21 06:56:59</t>
+  </si>
+  <si>
+    <t> 2018.06.20 03:29:39</t>
+  </si>
+  <si>
+    <t>D-H2PVND-VND-61681746</t>
+  </si>
+  <si>
+    <t> 2018.06.20 06:04:53</t>
+  </si>
+  <si>
+    <t> 2018.06.21 06:31:29</t>
+  </si>
+  <si>
+    <t> 2018.06.20 15:23:02</t>
+  </si>
+  <si>
+    <t> 2018.06.21 12:49:49</t>
+  </si>
+  <si>
+    <t> 2018.06.21 06:31:38</t>
+  </si>
+  <si>
+    <t> 2018.06.21 09:19:04</t>
+  </si>
+  <si>
+    <t> 2018.06.21 08:44:01</t>
+  </si>
+  <si>
+    <t> 2018.06.21 12:49:24</t>
+  </si>
+  <si>
+    <t> 2018.06.21 11:21:46</t>
+  </si>
+  <si>
+    <t> 2018.06.21 13:25:52</t>
+  </si>
+  <si>
+    <t> 2018.06.21 20:15:10</t>
+  </si>
+  <si>
+    <t> 2018.06.22 14:20:35</t>
+  </si>
+  <si>
+    <t> 2018.06.22 01:49:46</t>
+  </si>
+  <si>
+    <t> 2018.06.22 14:20:23</t>
+  </si>
+  <si>
+    <t> 2018.06.22 09:26:32</t>
+  </si>
+  <si>
+    <t> 2018.06.22 14:33:01</t>
+  </si>
+  <si>
+    <t> 2018.06.25 00:29:15</t>
+  </si>
+  <si>
+    <t> 2018.06.29 16:09:18</t>
+  </si>
+  <si>
+    <t> 2018.06.27 06:12:44</t>
+  </si>
+  <si>
+    <t> 2018.06.27 06:12:58</t>
+  </si>
+  <si>
+    <t> 2018.06.27 06:13:17</t>
+  </si>
+  <si>
+    <t> 2018.06.29 15:44:04</t>
+  </si>
+  <si>
+    <t> 2018.06.27 20:33:17</t>
+  </si>
+  <si>
+    <t> 2018.06.29 04:41:35</t>
+  </si>
+  <si>
+    <t> 2018.06.29 06:22:14</t>
+  </si>
+  <si>
+    <t>W-H2PVND-VND-62249801</t>
+  </si>
+  <si>
+    <t>Deposit/Withdrawal: 2 182.66</t>
+  </si>
+  <si>
+    <t>J</t>
   </si>
 </sst>
 </file>
@@ -375,17 +615,17 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="[$$-409]#,##0.00_);[Red]\([$$-409]#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00&quot;%&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00_);[Red]\([$$-409]#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00&quot;%&quot;"/>
   </numFmts>
   <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -425,7 +665,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -444,7 +684,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -738,9 +978,9 @@
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -814,55 +1054,124 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="7" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="180" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="12" fillId="4" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="180" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="10" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="12" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="7" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="7" fillId="5" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="4" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -870,7 +1179,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
-  <dxfs count="41">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -886,55 +1195,6 @@
         <vertical/>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color rgb="FF1AA631"/>
-      </font>
-      <fill>
-        <patternFill patternType="gray0625">
-          <fgColor rgb="FF0F22B1"/>
-        </patternFill>
-      </fill>
-      <border>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <font>
@@ -955,364 +1215,6 @@
         <patternFill patternType="lightUp">
           <fgColor theme="7" tint="0.39994506668294322"/>
           <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="7" tint="0.39994506668294322"/>
-          <bgColor auto="1"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="5" tint="0.79995117038483843"/>
-          <bgColor theme="7" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightUp">
-          <fgColor theme="4" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79995117038483843"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="5" tint="0.79998168889431442"/>
-          <bgColor theme="7" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF0F22B1"/>
-      </font>
-      <fill>
-        <patternFill patternType="lightGrid">
-          <fgColor theme="9" tint="0.59996337778862885"/>
-          <bgColor theme="9" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B0F0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1591,7 +1493,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1603,27 +1505,27 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="10.5" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="10.42578125" style="18" customWidth="1"/>
     <col min="3" max="8" width="14" style="18" customWidth="1"/>
-    <col min="9" max="9" width="11.625" style="18" customWidth="1"/>
-    <col min="10" max="16384" width="9.125" style="18"/>
+    <col min="9" max="9" width="11.5703125" style="18" customWidth="1"/>
+    <col min="10" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="40" t="s">
         <v>104</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="50"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
+      <c r="H2" s="41"/>
+      <c r="I2" s="41"/>
+      <c r="J2" s="42"/>
     </row>
     <row r="3" spans="2:10">
       <c r="B3" s="26" t="s">
@@ -1645,20 +1547,20 @@
         <v>106</v>
       </c>
       <c r="H3" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="I3" s="44" t="s">
         <v>108</v>
       </c>
-      <c r="I3" s="52" t="s">
-        <v>109</v>
-      </c>
-      <c r="J3" s="52" t="s">
-        <v>111</v>
+      <c r="J3" s="44" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="4" spans="2:10">
       <c r="B4" s="28">
         <v>43101</v>
       </c>
-      <c r="C4" s="51">
+      <c r="C4" s="43">
         <v>881.13</v>
       </c>
       <c r="D4" s="29">
@@ -1671,11 +1573,11 @@
         <v>0</v>
       </c>
       <c r="G4" s="29">
-        <f>C4+D4+F4-E4</f>
+        <f t="shared" ref="G4:G10" si="0">C4+D4+F4-E4</f>
         <v>881.13</v>
       </c>
       <c r="H4" s="39">
-        <f>(F4/C4)*100</f>
+        <f t="shared" ref="H4:H10" si="1">(F4/C4)*100</f>
         <v>0</v>
       </c>
       <c r="I4" s="29">
@@ -1700,11 +1602,11 @@
         <v>40.92</v>
       </c>
       <c r="G5" s="29">
-        <f>C5+D5+F5-E5</f>
+        <f t="shared" si="0"/>
         <v>1322.0500000000002</v>
       </c>
       <c r="H5" s="39">
-        <f>(F5/C5)*100</f>
+        <f t="shared" si="1"/>
         <v>4.6440366347757989</v>
       </c>
       <c r="I5" s="29">
@@ -1730,11 +1632,11 @@
         <v>0</v>
       </c>
       <c r="G6" s="29">
-        <f>C6+D6+F6-E6</f>
+        <f t="shared" si="0"/>
         <v>1322.0500000000002</v>
       </c>
       <c r="H6" s="39">
-        <f>(F6/C6)*100</f>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="I6" s="29">
@@ -1760,11 +1662,11 @@
         <v>119.16</v>
       </c>
       <c r="G7" s="29">
-        <f>C7+D7+F7-E7</f>
+        <f t="shared" si="0"/>
         <v>1441.2100000000003</v>
       </c>
       <c r="H7" s="39">
-        <f>(F7/C7)*100</f>
+        <f t="shared" si="1"/>
         <v>9.0132748383192762</v>
       </c>
       <c r="I7" s="29">
@@ -1790,11 +1692,11 @@
         <v>745.39</v>
       </c>
       <c r="G8" s="29">
-        <f>C8+D8+F8-E8</f>
+        <f t="shared" si="0"/>
         <v>2734.4100000000003</v>
       </c>
       <c r="H8" s="39">
-        <f>(F8/C8)*100</f>
+        <f t="shared" si="1"/>
         <v>51.71973550003122</v>
       </c>
       <c r="I8" s="29">
@@ -1820,11 +1722,11 @@
         <v>726.18</v>
       </c>
       <c r="G9" s="29">
-        <f>C9+D9+F9-E9</f>
+        <f t="shared" si="0"/>
         <v>3890.13</v>
       </c>
       <c r="H9" s="39">
-        <f>(F9/C9)*100</f>
+        <f t="shared" si="1"/>
         <v>26.557100069119109</v>
       </c>
       <c r="I9" s="29">
@@ -1850,11 +1752,11 @@
         <v>262.44</v>
       </c>
       <c r="G10" s="29">
-        <f>C10+D10+F10-E10</f>
+        <f t="shared" si="0"/>
         <v>4152.57</v>
       </c>
       <c r="H10" s="39">
-        <f>(F10/C10)*100</f>
+        <f t="shared" si="1"/>
         <v>6.7463041080889328</v>
       </c>
       <c r="I10" s="31">
@@ -2029,7 +1931,7 @@
     </row>
     <row r="22" spans="2:10">
       <c r="B22" s="26" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C22" s="36"/>
       <c r="D22" s="37">
@@ -2061,15 +1963,15 @@
   </sheetData>
   <phoneticPr fontId="9"/>
   <conditionalFormatting sqref="B4:J4 J5:J21">
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
+      <formula>"Fail"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="5" operator="equal">
       <formula>"Pass"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="equal">
-      <formula>"Fail"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G10">
-    <cfRule type="aboveAverage" dxfId="3" priority="3"/>
+    <cfRule type="aboveAverage" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4">
     <cfRule type="colorScale" priority="1">
@@ -2096,36 +1998,38 @@
   <sheetPr filterMode="1"/>
   <dimension ref="B1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B36" sqref="B36"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="13.125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="13.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="18" customWidth="1"/>
     <col min="5" max="5" width="17" style="18" customWidth="1"/>
-    <col min="6" max="7" width="13.125" style="18" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="18"/>
+    <col min="6" max="7" width="13.140625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="40"/>
-      <c r="G1" s="40"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="25" t="s">
@@ -2512,13 +2416,1529 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:14" s="1" customFormat="1" ht="23.25" thickBot="1">
+      <c r="A1" s="61">
+        <v>43252</v>
+      </c>
+      <c r="B1" s="62" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="63" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>69</v>
+      </c>
+      <c r="E1" s="63" t="s">
+        <v>68</v>
+      </c>
+      <c r="F1" s="63" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="H1" s="63" t="s">
+        <v>66</v>
+      </c>
+      <c r="I1" s="63" t="s">
+        <v>65</v>
+      </c>
+      <c r="J1" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="K1" s="63" t="s">
+        <v>63</v>
+      </c>
+      <c r="L1" s="63" t="s">
+        <v>62</v>
+      </c>
+      <c r="M1" s="63" t="s">
+        <v>61</v>
+      </c>
+      <c r="N1" s="64" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B2" s="65">
+        <v>130907515</v>
+      </c>
+      <c r="C2" s="54" t="s">
+        <v>112</v>
+      </c>
+      <c r="D2" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="58" t="s">
+        <v>113</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="58"/>
+      <c r="I2" s="58"/>
+      <c r="J2" s="58"/>
+      <c r="K2" s="58"/>
+      <c r="L2" s="58"/>
+      <c r="M2" s="58"/>
+      <c r="N2" s="66" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B3" s="67">
+        <v>137714682</v>
+      </c>
+      <c r="C3" s="56" t="s">
+        <v>115</v>
+      </c>
+      <c r="D3" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="F3" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="G3" s="55">
+        <v>147.316</v>
+      </c>
+      <c r="H3" s="55">
+        <v>0</v>
+      </c>
+      <c r="I3" s="55">
+        <v>0</v>
+      </c>
+      <c r="J3" s="56" t="s">
+        <v>116</v>
+      </c>
+      <c r="K3" s="55">
+        <v>147.66900000000001</v>
+      </c>
+      <c r="L3" s="55">
+        <v>0</v>
+      </c>
+      <c r="M3" s="55">
+        <v>-0.4</v>
+      </c>
+      <c r="N3" s="68">
+        <v>31.93</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B4" s="65">
+        <v>137763688</v>
+      </c>
+      <c r="C4" s="54" t="s">
+        <v>117</v>
+      </c>
+      <c r="D4" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="F4" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G4" s="53">
+        <v>1.93411</v>
+      </c>
+      <c r="H4" s="53">
+        <v>0</v>
+      </c>
+      <c r="I4" s="53">
+        <v>0</v>
+      </c>
+      <c r="J4" s="54" t="s">
+        <v>118</v>
+      </c>
+      <c r="K4" s="53">
+        <v>1.93946</v>
+      </c>
+      <c r="L4" s="53">
+        <v>0</v>
+      </c>
+      <c r="M4" s="53">
+        <v>-21.8</v>
+      </c>
+      <c r="N4" s="69">
+        <v>36.47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B5" s="67">
+        <v>138022429</v>
+      </c>
+      <c r="C5" s="56" t="s">
+        <v>119</v>
+      </c>
+      <c r="D5" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="F5" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="G5" s="55">
+        <v>1.51084</v>
+      </c>
+      <c r="H5" s="55">
+        <v>0</v>
+      </c>
+      <c r="I5" s="55">
+        <v>0</v>
+      </c>
+      <c r="J5" s="56" t="s">
+        <v>121</v>
+      </c>
+      <c r="K5" s="55">
+        <v>1.5121899999999999</v>
+      </c>
+      <c r="L5" s="55">
+        <v>0</v>
+      </c>
+      <c r="M5" s="55">
+        <v>-1.66</v>
+      </c>
+      <c r="N5" s="68">
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B6" s="65">
+        <v>138393922</v>
+      </c>
+      <c r="C6" s="54" t="s">
+        <v>122</v>
+      </c>
+      <c r="D6" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="53">
+        <v>0.08</v>
+      </c>
+      <c r="F6" s="53" t="s">
+        <v>123</v>
+      </c>
+      <c r="G6" s="53">
+        <v>0.70413000000000003</v>
+      </c>
+      <c r="H6" s="53">
+        <v>0</v>
+      </c>
+      <c r="I6" s="53">
+        <v>0</v>
+      </c>
+      <c r="J6" s="54" t="s">
+        <v>124</v>
+      </c>
+      <c r="K6" s="53">
+        <v>0.70118000000000003</v>
+      </c>
+      <c r="L6" s="53">
+        <v>0</v>
+      </c>
+      <c r="M6" s="53">
+        <v>-0.22</v>
+      </c>
+      <c r="N6" s="69">
+        <v>23.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B7" s="67">
+        <v>138461980</v>
+      </c>
+      <c r="C7" s="56" t="s">
+        <v>125</v>
+      </c>
+      <c r="D7" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="59" t="s">
+        <v>126</v>
+      </c>
+      <c r="F7" s="59"/>
+      <c r="G7" s="59"/>
+      <c r="H7" s="59"/>
+      <c r="I7" s="59"/>
+      <c r="J7" s="59"/>
+      <c r="K7" s="59"/>
+      <c r="L7" s="59"/>
+      <c r="M7" s="59"/>
+      <c r="N7" s="70">
+        <v>-100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B8" s="65">
+        <v>138475841</v>
+      </c>
+      <c r="C8" s="54" t="s">
+        <v>127</v>
+      </c>
+      <c r="D8" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E8" s="53">
+        <v>0.06</v>
+      </c>
+      <c r="F8" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="G8" s="53">
+        <v>1.6656299999999999</v>
+      </c>
+      <c r="H8" s="53">
+        <v>0</v>
+      </c>
+      <c r="I8" s="53">
+        <v>0</v>
+      </c>
+      <c r="J8" s="54" t="s">
+        <v>129</v>
+      </c>
+      <c r="K8" s="53">
+        <v>1.67709</v>
+      </c>
+      <c r="L8" s="53">
+        <v>0</v>
+      </c>
+      <c r="M8" s="53">
+        <v>-2.39</v>
+      </c>
+      <c r="N8" s="69">
+        <v>48.47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B9" s="67">
+        <v>138654225</v>
+      </c>
+      <c r="C9" s="56" t="s">
+        <v>130</v>
+      </c>
+      <c r="D9" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E9" s="55">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G9" s="55">
+        <v>1.6786099999999999</v>
+      </c>
+      <c r="H9" s="55">
+        <v>0</v>
+      </c>
+      <c r="I9" s="55">
+        <v>0</v>
+      </c>
+      <c r="J9" s="56" t="s">
+        <v>131</v>
+      </c>
+      <c r="K9" s="55">
+        <v>1.6778999999999999</v>
+      </c>
+      <c r="L9" s="55">
+        <v>0</v>
+      </c>
+      <c r="M9" s="55">
+        <v>0</v>
+      </c>
+      <c r="N9" s="68">
+        <v>2.4900000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B10" s="65">
+        <v>138723413</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>132</v>
+      </c>
+      <c r="D10" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="58" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="58"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="58"/>
+      <c r="I10" s="58"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="58"/>
+      <c r="L10" s="58"/>
+      <c r="M10" s="58"/>
+      <c r="N10" s="66">
+        <v>-20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B11" s="67">
+        <v>138732442</v>
+      </c>
+      <c r="C11" s="56" t="s">
+        <v>134</v>
+      </c>
+      <c r="D11" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" s="55">
+        <v>0.01</v>
+      </c>
+      <c r="F11" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G11" s="55">
+        <v>1.90551</v>
+      </c>
+      <c r="H11" s="55">
+        <v>0</v>
+      </c>
+      <c r="I11" s="55">
+        <v>0</v>
+      </c>
+      <c r="J11" s="56" t="s">
+        <v>135</v>
+      </c>
+      <c r="K11" s="55">
+        <v>1.90669</v>
+      </c>
+      <c r="L11" s="55">
+        <v>0</v>
+      </c>
+      <c r="M11" s="55">
+        <v>-0.4</v>
+      </c>
+      <c r="N11" s="68">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B12" s="65">
+        <v>138736541</v>
+      </c>
+      <c r="C12" s="54" t="s">
+        <v>136</v>
+      </c>
+      <c r="D12" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E12" s="53">
+        <v>0.12</v>
+      </c>
+      <c r="F12" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="53">
+        <v>1.9080299999999999</v>
+      </c>
+      <c r="H12" s="53">
+        <v>0</v>
+      </c>
+      <c r="I12" s="53">
+        <v>0</v>
+      </c>
+      <c r="J12" s="54" t="s">
+        <v>137</v>
+      </c>
+      <c r="K12" s="53">
+        <v>1.9093899999999999</v>
+      </c>
+      <c r="L12" s="53">
+        <v>0</v>
+      </c>
+      <c r="M12" s="53">
+        <v>-4.54</v>
+      </c>
+      <c r="N12" s="69">
+        <v>11.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B13" s="67">
+        <v>138897659</v>
+      </c>
+      <c r="C13" s="56" t="s">
+        <v>138</v>
+      </c>
+      <c r="D13" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" s="55">
+        <v>0.12</v>
+      </c>
+      <c r="F13" s="55" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="55">
+        <v>1.3014600000000001</v>
+      </c>
+      <c r="H13" s="55">
+        <v>0</v>
+      </c>
+      <c r="I13" s="55">
+        <v>0</v>
+      </c>
+      <c r="J13" s="56" t="s">
+        <v>139</v>
+      </c>
+      <c r="K13" s="55">
+        <v>1.29772</v>
+      </c>
+      <c r="L13" s="55">
+        <v>0</v>
+      </c>
+      <c r="M13" s="55">
+        <v>-0.88</v>
+      </c>
+      <c r="N13" s="68">
+        <v>34.58</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B14" s="65">
+        <v>138953312</v>
+      </c>
+      <c r="C14" s="54" t="s">
+        <v>140</v>
+      </c>
+      <c r="D14" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E14" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="F14" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G14" s="53">
+        <v>147.58099999999999</v>
+      </c>
+      <c r="H14" s="53">
+        <v>0</v>
+      </c>
+      <c r="I14" s="53">
+        <v>0</v>
+      </c>
+      <c r="J14" s="54" t="s">
+        <v>141</v>
+      </c>
+      <c r="K14" s="53">
+        <v>147.79400000000001</v>
+      </c>
+      <c r="L14" s="53">
+        <v>0</v>
+      </c>
+      <c r="M14" s="53">
+        <v>0</v>
+      </c>
+      <c r="N14" s="69">
+        <v>9.68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B15" s="67">
+        <v>138963274</v>
+      </c>
+      <c r="C15" s="56" t="s">
+        <v>142</v>
+      </c>
+      <c r="D15" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E15" s="55">
+        <v>0.05</v>
+      </c>
+      <c r="F15" s="55" t="s">
+        <v>143</v>
+      </c>
+      <c r="G15" s="55">
+        <v>111.79300000000001</v>
+      </c>
+      <c r="H15" s="55">
+        <v>0</v>
+      </c>
+      <c r="I15" s="55">
+        <v>0</v>
+      </c>
+      <c r="J15" s="56" t="s">
+        <v>144</v>
+      </c>
+      <c r="K15" s="55">
+        <v>111.069</v>
+      </c>
+      <c r="L15" s="55">
+        <v>0</v>
+      </c>
+      <c r="M15" s="55">
+        <v>0</v>
+      </c>
+      <c r="N15" s="68">
+        <v>32.78</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B16" s="65">
+        <v>139069945</v>
+      </c>
+      <c r="C16" s="54" t="s">
+        <v>145</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="53">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="F16" s="53" t="s">
+        <v>120</v>
+      </c>
+      <c r="G16" s="53">
+        <v>1.52217</v>
+      </c>
+      <c r="H16" s="53">
+        <v>0</v>
+      </c>
+      <c r="I16" s="53">
+        <v>0</v>
+      </c>
+      <c r="J16" s="54" t="s">
+        <v>146</v>
+      </c>
+      <c r="K16" s="53">
+        <v>1.5281100000000001</v>
+      </c>
+      <c r="L16" s="53">
+        <v>0</v>
+      </c>
+      <c r="M16" s="53">
+        <v>0</v>
+      </c>
+      <c r="N16" s="69">
+        <v>-31.59</v>
+      </c>
+    </row>
+    <row r="17" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B17" s="67">
+        <v>139070001</v>
+      </c>
+      <c r="C17" s="56" t="s">
+        <v>147</v>
+      </c>
+      <c r="D17" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E17" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="F17" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G17" s="55">
+        <v>1.90944</v>
+      </c>
+      <c r="H17" s="55">
+        <v>0</v>
+      </c>
+      <c r="I17" s="55">
+        <v>0</v>
+      </c>
+      <c r="J17" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="K17" s="55">
+        <v>1.9113</v>
+      </c>
+      <c r="L17" s="55">
+        <v>0</v>
+      </c>
+      <c r="M17" s="55">
+        <v>0</v>
+      </c>
+      <c r="N17" s="68">
+        <v>-7.75</v>
+      </c>
+    </row>
+    <row r="18" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B18" s="65">
+        <v>139076560</v>
+      </c>
+      <c r="C18" s="54" t="s">
+        <v>149</v>
+      </c>
+      <c r="D18" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E18" s="53">
+        <v>0.13</v>
+      </c>
+      <c r="F18" s="53" t="s">
+        <v>128</v>
+      </c>
+      <c r="G18" s="53">
+        <v>1.66998</v>
+      </c>
+      <c r="H18" s="53">
+        <v>0</v>
+      </c>
+      <c r="I18" s="53">
+        <v>0</v>
+      </c>
+      <c r="J18" s="54" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" s="53">
+        <v>1.67113</v>
+      </c>
+      <c r="L18" s="53">
+        <v>0</v>
+      </c>
+      <c r="M18" s="53">
+        <v>0</v>
+      </c>
+      <c r="N18" s="69">
+        <v>10.39</v>
+      </c>
+    </row>
+    <row r="19" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B19" s="67">
+        <v>139121598</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>151</v>
+      </c>
+      <c r="D19" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E19" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="F19" s="55" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="55">
+        <v>1.67015</v>
+      </c>
+      <c r="H19" s="55">
+        <v>0</v>
+      </c>
+      <c r="I19" s="55">
+        <v>0</v>
+      </c>
+      <c r="J19" s="56" t="s">
+        <v>152</v>
+      </c>
+      <c r="K19" s="55">
+        <v>1.6797599999999999</v>
+      </c>
+      <c r="L19" s="55">
+        <v>0</v>
+      </c>
+      <c r="M19" s="55">
+        <v>-0.97</v>
+      </c>
+      <c r="N19" s="68">
+        <v>66.22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B20" s="65">
+        <v>139177488</v>
+      </c>
+      <c r="C20" s="54" t="s">
+        <v>153</v>
+      </c>
+      <c r="D20" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E20" s="53">
+        <v>0.06</v>
+      </c>
+      <c r="F20" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="G20" s="53">
+        <v>1.7922199999999999</v>
+      </c>
+      <c r="H20" s="53">
+        <v>0</v>
+      </c>
+      <c r="I20" s="53">
+        <v>0</v>
+      </c>
+      <c r="J20" s="54" t="s">
+        <v>155</v>
+      </c>
+      <c r="K20" s="53">
+        <v>1.79392</v>
+      </c>
+      <c r="L20" s="53">
+        <v>0</v>
+      </c>
+      <c r="M20" s="53">
+        <v>0</v>
+      </c>
+      <c r="N20" s="69">
+        <v>7.51</v>
+      </c>
+    </row>
+    <row r="21" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B21" s="67">
+        <v>139189288</v>
+      </c>
+      <c r="C21" s="56" t="s">
+        <v>156</v>
+      </c>
+      <c r="D21" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E21" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="F21" s="55" t="s">
+        <v>154</v>
+      </c>
+      <c r="G21" s="55">
+        <v>1.79284</v>
+      </c>
+      <c r="H21" s="55">
+        <v>0</v>
+      </c>
+      <c r="I21" s="55">
+        <v>0</v>
+      </c>
+      <c r="J21" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="K21" s="55">
+        <v>1.78762</v>
+      </c>
+      <c r="L21" s="55">
+        <v>0</v>
+      </c>
+      <c r="M21" s="55">
+        <v>0</v>
+      </c>
+      <c r="N21" s="68">
+        <v>23.07</v>
+      </c>
+    </row>
+    <row r="22" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B22" s="65">
+        <v>139193605</v>
+      </c>
+      <c r="C22" s="54" t="s">
+        <v>158</v>
+      </c>
+      <c r="D22" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="F22" s="53" t="s">
+        <v>154</v>
+      </c>
+      <c r="G22" s="53">
+        <v>1.7907599999999999</v>
+      </c>
+      <c r="H22" s="53">
+        <v>0</v>
+      </c>
+      <c r="I22" s="53">
+        <v>0</v>
+      </c>
+      <c r="J22" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="K22" s="53">
+        <v>1.7876399999999999</v>
+      </c>
+      <c r="L22" s="53">
+        <v>0</v>
+      </c>
+      <c r="M22" s="53">
+        <v>0</v>
+      </c>
+      <c r="N22" s="69">
+        <v>11.49</v>
+      </c>
+    </row>
+    <row r="23" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B23" s="67">
+        <v>139209052</v>
+      </c>
+      <c r="C23" s="56" t="s">
+        <v>160</v>
+      </c>
+      <c r="D23" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E23" s="55">
+        <v>0.1</v>
+      </c>
+      <c r="F23" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="G23" s="55">
+        <v>144.608</v>
+      </c>
+      <c r="H23" s="55">
+        <v>0</v>
+      </c>
+      <c r="I23" s="55">
+        <v>0</v>
+      </c>
+      <c r="J23" s="56" t="s">
+        <v>161</v>
+      </c>
+      <c r="K23" s="55">
+        <v>145.274</v>
+      </c>
+      <c r="L23" s="55">
+        <v>0</v>
+      </c>
+      <c r="M23" s="55">
+        <v>-0.08</v>
+      </c>
+      <c r="N23" s="68">
+        <v>60.22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B24" s="65">
+        <v>139249180</v>
+      </c>
+      <c r="C24" s="54" t="s">
+        <v>162</v>
+      </c>
+      <c r="D24" s="53" t="s">
+        <v>4</v>
+      </c>
+      <c r="E24" s="58" t="s">
+        <v>163</v>
+      </c>
+      <c r="F24" s="58"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="58"/>
+      <c r="I24" s="58"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="58"/>
+      <c r="L24" s="58"/>
+      <c r="M24" s="58"/>
+      <c r="N24" s="66">
+        <v>699.54</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B25" s="67">
+        <v>139254304</v>
+      </c>
+      <c r="C25" s="56" t="s">
+        <v>164</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E25" s="55">
+        <v>0.06</v>
+      </c>
+      <c r="F25" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G25" s="55">
+        <v>1.9072100000000001</v>
+      </c>
+      <c r="H25" s="55">
+        <v>0</v>
+      </c>
+      <c r="I25" s="55">
+        <v>0</v>
+      </c>
+      <c r="J25" s="56" t="s">
+        <v>165</v>
+      </c>
+      <c r="K25" s="55">
+        <v>1.9213800000000001</v>
+      </c>
+      <c r="L25" s="55">
+        <v>0</v>
+      </c>
+      <c r="M25" s="55">
+        <v>-1.0900000000000001</v>
+      </c>
+      <c r="N25" s="68">
+        <v>58.1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B26" s="65">
+        <v>139288612</v>
+      </c>
+      <c r="C26" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="D26" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E26" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="F26" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G26" s="53">
+        <v>145.35</v>
+      </c>
+      <c r="H26" s="53">
+        <v>0</v>
+      </c>
+      <c r="I26" s="53">
+        <v>0</v>
+      </c>
+      <c r="J26" s="54" t="s">
+        <v>167</v>
+      </c>
+      <c r="K26" s="53">
+        <v>146.04</v>
+      </c>
+      <c r="L26" s="53">
+        <v>0</v>
+      </c>
+      <c r="M26" s="53">
+        <v>-0.03</v>
+      </c>
+      <c r="N26" s="69">
+        <v>31.29</v>
+      </c>
+    </row>
+    <row r="27" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B27" s="67">
+        <v>139320132</v>
+      </c>
+      <c r="C27" s="56" t="s">
+        <v>168</v>
+      </c>
+      <c r="D27" s="55" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="55">
+        <v>0.05</v>
+      </c>
+      <c r="F27" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="55">
+        <v>1.9212400000000001</v>
+      </c>
+      <c r="H27" s="55">
+        <v>0</v>
+      </c>
+      <c r="I27" s="55">
+        <v>0</v>
+      </c>
+      <c r="J27" s="56" t="s">
+        <v>169</v>
+      </c>
+      <c r="K27" s="55">
+        <v>1.91825</v>
+      </c>
+      <c r="L27" s="55">
+        <v>0</v>
+      </c>
+      <c r="M27" s="55">
+        <v>0</v>
+      </c>
+      <c r="N27" s="68">
+        <v>10.23</v>
+      </c>
+    </row>
+    <row r="28" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B28" s="65">
+        <v>139321846</v>
+      </c>
+      <c r="C28" s="54" t="s">
+        <v>170</v>
+      </c>
+      <c r="D28" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E28" s="53">
+        <v>0.13</v>
+      </c>
+      <c r="F28" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G28" s="53">
+        <v>145</v>
+      </c>
+      <c r="H28" s="53">
+        <v>0</v>
+      </c>
+      <c r="I28" s="53">
+        <v>0</v>
+      </c>
+      <c r="J28" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="K28" s="53">
+        <v>146.07</v>
+      </c>
+      <c r="L28" s="53">
+        <v>0</v>
+      </c>
+      <c r="M28" s="53">
+        <v>0</v>
+      </c>
+      <c r="N28" s="69">
+        <v>126.17</v>
+      </c>
+    </row>
+    <row r="29" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B29" s="67">
+        <v>139344009</v>
+      </c>
+      <c r="C29" s="56" t="s">
+        <v>172</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E29" s="55">
+        <v>0.05</v>
+      </c>
+      <c r="F29" s="55" t="s">
+        <v>16</v>
+      </c>
+      <c r="G29" s="55">
+        <v>1.9267300000000001</v>
+      </c>
+      <c r="H29" s="55">
+        <v>0</v>
+      </c>
+      <c r="I29" s="55">
+        <v>0</v>
+      </c>
+      <c r="J29" s="56" t="s">
+        <v>173</v>
+      </c>
+      <c r="K29" s="55">
+        <v>1.9274500000000001</v>
+      </c>
+      <c r="L29" s="55">
+        <v>0</v>
+      </c>
+      <c r="M29" s="55">
+        <v>0</v>
+      </c>
+      <c r="N29" s="68">
+        <v>2.48</v>
+      </c>
+    </row>
+    <row r="30" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B30" s="65">
+        <v>139373451</v>
+      </c>
+      <c r="C30" s="54" t="s">
+        <v>174</v>
+      </c>
+      <c r="D30" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E30" s="53">
+        <v>0.1</v>
+      </c>
+      <c r="F30" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G30" s="53">
+        <v>145.71899999999999</v>
+      </c>
+      <c r="H30" s="53">
+        <v>0</v>
+      </c>
+      <c r="I30" s="53">
+        <v>0</v>
+      </c>
+      <c r="J30" s="54" t="s">
+        <v>175</v>
+      </c>
+      <c r="K30" s="53">
+        <v>146.01400000000001</v>
+      </c>
+      <c r="L30" s="53">
+        <v>0</v>
+      </c>
+      <c r="M30" s="53">
+        <v>-0.02</v>
+      </c>
+      <c r="N30" s="69">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B31" s="67">
+        <v>139381854</v>
+      </c>
+      <c r="C31" s="56" t="s">
+        <v>176</v>
+      </c>
+      <c r="D31" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E31" s="55">
+        <v>0.08</v>
+      </c>
+      <c r="F31" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="G31" s="55">
+        <v>145.947</v>
+      </c>
+      <c r="H31" s="55">
+        <v>0</v>
+      </c>
+      <c r="I31" s="55">
+        <v>0</v>
+      </c>
+      <c r="J31" s="56" t="s">
+        <v>177</v>
+      </c>
+      <c r="K31" s="55">
+        <v>146.01</v>
+      </c>
+      <c r="L31" s="55">
+        <v>0</v>
+      </c>
+      <c r="M31" s="55">
+        <v>0</v>
+      </c>
+      <c r="N31" s="68">
+        <v>4.58</v>
+      </c>
+    </row>
+    <row r="32" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B32" s="65">
+        <v>139407314</v>
+      </c>
+      <c r="C32" s="54" t="s">
+        <v>178</v>
+      </c>
+      <c r="D32" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E32" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="F32" s="53" t="s">
+        <v>13</v>
+      </c>
+      <c r="G32" s="53">
+        <v>1.32681</v>
+      </c>
+      <c r="H32" s="53">
+        <v>0</v>
+      </c>
+      <c r="I32" s="53">
+        <v>0</v>
+      </c>
+      <c r="J32" s="54" t="s">
+        <v>179</v>
+      </c>
+      <c r="K32" s="53">
+        <v>1.33399</v>
+      </c>
+      <c r="L32" s="53">
+        <v>0</v>
+      </c>
+      <c r="M32" s="53">
+        <v>0</v>
+      </c>
+      <c r="N32" s="69">
+        <v>-26.91</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B33" s="67">
+        <v>139426625</v>
+      </c>
+      <c r="C33" s="56" t="s">
+        <v>180</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="55">
+        <v>0.2</v>
+      </c>
+      <c r="F33" s="55" t="s">
+        <v>37</v>
+      </c>
+      <c r="G33" s="55">
+        <v>145.5</v>
+      </c>
+      <c r="H33" s="55">
+        <v>0</v>
+      </c>
+      <c r="I33" s="55">
+        <v>0</v>
+      </c>
+      <c r="J33" s="56" t="s">
+        <v>181</v>
+      </c>
+      <c r="K33" s="55">
+        <v>146.16900000000001</v>
+      </c>
+      <c r="L33" s="55">
+        <v>0</v>
+      </c>
+      <c r="M33" s="55">
+        <v>-0.23</v>
+      </c>
+      <c r="N33" s="68">
+        <v>120.79</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B34" s="65">
+        <v>139619569</v>
+      </c>
+      <c r="C34" s="54" t="s">
+        <v>182</v>
+      </c>
+      <c r="D34" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="E34" s="53">
+        <v>0.08</v>
+      </c>
+      <c r="F34" s="53" t="s">
+        <v>58</v>
+      </c>
+      <c r="G34" s="53">
+        <v>1.16625</v>
+      </c>
+      <c r="H34" s="53">
+        <v>0</v>
+      </c>
+      <c r="I34" s="53">
+        <v>0</v>
+      </c>
+      <c r="J34" s="54" t="s">
+        <v>183</v>
+      </c>
+      <c r="K34" s="53">
+        <v>1.16649</v>
+      </c>
+      <c r="L34" s="53">
+        <v>0</v>
+      </c>
+      <c r="M34" s="53">
+        <v>0</v>
+      </c>
+      <c r="N34" s="69">
+        <v>-1.92</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B35" s="67">
+        <v>139619621</v>
+      </c>
+      <c r="C35" s="56" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E35" s="55">
+        <v>0.08</v>
+      </c>
+      <c r="F35" s="55" t="s">
+        <v>58</v>
+      </c>
+      <c r="G35" s="55">
+        <v>1.1663300000000001</v>
+      </c>
+      <c r="H35" s="55">
+        <v>0</v>
+      </c>
+      <c r="I35" s="55">
+        <v>0</v>
+      </c>
+      <c r="J35" s="56" t="s">
+        <v>185</v>
+      </c>
+      <c r="K35" s="55">
+        <v>1.16723</v>
+      </c>
+      <c r="L35" s="55">
+        <v>0</v>
+      </c>
+      <c r="M35" s="55">
+        <v>-2.87</v>
+      </c>
+      <c r="N35" s="68">
+        <v>7.2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B36" s="65">
+        <v>139682129</v>
+      </c>
+      <c r="C36" s="54" t="s">
+        <v>186</v>
+      </c>
+      <c r="D36" s="53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E36" s="53">
+        <v>0.05</v>
+      </c>
+      <c r="F36" s="53" t="s">
+        <v>37</v>
+      </c>
+      <c r="G36" s="53">
+        <v>144.619</v>
+      </c>
+      <c r="H36" s="53">
+        <v>0</v>
+      </c>
+      <c r="I36" s="53">
+        <v>0</v>
+      </c>
+      <c r="J36" s="54" t="s">
+        <v>187</v>
+      </c>
+      <c r="K36" s="53">
+        <v>145.21700000000001</v>
+      </c>
+      <c r="L36" s="53">
+        <v>0</v>
+      </c>
+      <c r="M36" s="53">
+        <v>-0.04</v>
+      </c>
+      <c r="N36" s="69">
+        <v>27.01</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B37" s="67">
+        <v>139780262</v>
+      </c>
+      <c r="C37" s="56" t="s">
+        <v>188</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="59" t="s">
+        <v>189</v>
+      </c>
+      <c r="F37" s="59"/>
+      <c r="G37" s="59"/>
+      <c r="H37" s="59"/>
+      <c r="I37" s="59"/>
+      <c r="J37" s="59"/>
+      <c r="K37" s="59"/>
+      <c r="L37" s="59"/>
+      <c r="M37" s="59"/>
+      <c r="N37" s="70">
+        <v>-150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B38" s="71"/>
+      <c r="C38" s="60"/>
+      <c r="D38" s="60"/>
+      <c r="E38" s="60"/>
+      <c r="F38" s="60"/>
+      <c r="G38" s="60"/>
+      <c r="H38" s="60"/>
+      <c r="I38" s="60"/>
+      <c r="J38" s="60"/>
+      <c r="K38" s="60"/>
+      <c r="L38" s="57">
+        <v>0</v>
+      </c>
+      <c r="M38" s="57">
+        <v>-37.619999999999997</v>
+      </c>
+      <c r="N38" s="72">
+        <v>763.8</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" s="1" customFormat="1" ht="13.5">
+      <c r="B39" s="73" t="s">
+        <v>190</v>
+      </c>
+      <c r="C39" s="74"/>
+      <c r="D39" s="74"/>
+      <c r="E39" s="74"/>
+      <c r="F39" s="74" t="s">
+        <v>1</v>
+      </c>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="74"/>
+      <c r="J39" s="74"/>
+      <c r="K39" s="74" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="74"/>
+      <c r="M39" s="74">
+        <v>726.18</v>
+      </c>
+      <c r="N39" s="75"/>
+    </row>
+    <row r="40" spans="1:14">
+      <c r="A40" t="s">
+        <v>191</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B38:K38"/>
+    <mergeCell ref="B39:E39"/>
+    <mergeCell ref="F39:J39"/>
+    <mergeCell ref="K39:L39"/>
+    <mergeCell ref="M39:N39"/>
+    <mergeCell ref="E2:M2"/>
+    <mergeCell ref="E7:M7"/>
+    <mergeCell ref="E10:M10"/>
+    <mergeCell ref="E24:M24"/>
+    <mergeCell ref="E37:M37"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29:XFD67"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9.125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.5">
@@ -2698,17 +4118,17 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="41" t="s">
+      <c r="E5" s="52" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="41"/>
-      <c r="G5" s="41"/>
-      <c r="H5" s="41"/>
-      <c r="I5" s="41"/>
-      <c r="J5" s="41"/>
-      <c r="K5" s="41"/>
-      <c r="L5" s="41"/>
-      <c r="M5" s="41"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="52"/>
+      <c r="I5" s="52"/>
+      <c r="J5" s="52"/>
+      <c r="K5" s="52"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="52"/>
       <c r="N5" s="15">
         <v>-100</v>
       </c>
@@ -2723,17 +4143,17 @@
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="46" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="42"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="46"/>
+      <c r="I6" s="46"/>
+      <c r="J6" s="46"/>
+      <c r="K6" s="46"/>
+      <c r="L6" s="46"/>
+      <c r="M6" s="46"/>
       <c r="N6" s="16">
         <v>100</v>
       </c>
@@ -2830,17 +4250,17 @@
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="41" t="s">
+      <c r="E9" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="41"/>
-      <c r="G9" s="41"/>
-      <c r="H9" s="41"/>
-      <c r="I9" s="41"/>
-      <c r="J9" s="41"/>
-      <c r="K9" s="41"/>
-      <c r="L9" s="41"/>
-      <c r="M9" s="41"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="52"/>
+      <c r="H9" s="52"/>
+      <c r="I9" s="52"/>
+      <c r="J9" s="52"/>
+      <c r="K9" s="52"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="52"/>
       <c r="N9" s="15">
         <v>15.36</v>
       </c>
@@ -2896,17 +4316,17 @@
       <c r="D11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="41" t="s">
+      <c r="E11" s="52" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="41"/>
-      <c r="G11" s="41"/>
-      <c r="H11" s="41"/>
-      <c r="I11" s="41"/>
-      <c r="J11" s="41"/>
-      <c r="K11" s="41"/>
-      <c r="L11" s="41"/>
-      <c r="M11" s="41"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="52"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
       <c r="N11" s="15">
         <v>-20</v>
       </c>
@@ -3003,17 +4423,17 @@
       <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="46" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="42"/>
-      <c r="G14" s="42"/>
-      <c r="H14" s="42"/>
-      <c r="I14" s="42"/>
-      <c r="J14" s="42"/>
-      <c r="K14" s="42"/>
-      <c r="L14" s="42"/>
-      <c r="M14" s="42"/>
+      <c r="F14" s="46"/>
+      <c r="G14" s="46"/>
+      <c r="H14" s="46"/>
+      <c r="I14" s="46"/>
+      <c r="J14" s="46"/>
+      <c r="K14" s="46"/>
+      <c r="L14" s="46"/>
+      <c r="M14" s="46"/>
       <c r="N14" s="16">
         <v>-50</v>
       </c>
@@ -3069,17 +4489,17 @@
       <c r="D16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="42" t="s">
+      <c r="E16" s="46" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="42"/>
-      <c r="G16" s="42"/>
-      <c r="H16" s="42"/>
-      <c r="I16" s="42"/>
-      <c r="J16" s="42"/>
-      <c r="K16" s="42"/>
-      <c r="L16" s="42"/>
-      <c r="M16" s="42"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="46"/>
+      <c r="J16" s="46"/>
+      <c r="K16" s="46"/>
+      <c r="L16" s="46"/>
+      <c r="M16" s="46"/>
       <c r="N16" s="16">
         <v>-50</v>
       </c>
@@ -3135,17 +4555,17 @@
       <c r="D18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="42" t="s">
+      <c r="E18" s="46" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="42"/>
-      <c r="G18" s="42"/>
-      <c r="H18" s="42"/>
-      <c r="I18" s="42"/>
-      <c r="J18" s="42"/>
-      <c r="K18" s="42"/>
-      <c r="L18" s="42"/>
-      <c r="M18" s="42"/>
+      <c r="F18" s="46"/>
+      <c r="G18" s="46"/>
+      <c r="H18" s="46"/>
+      <c r="I18" s="46"/>
+      <c r="J18" s="46"/>
+      <c r="K18" s="46"/>
+      <c r="L18" s="46"/>
+      <c r="M18" s="46"/>
       <c r="N18" s="16">
         <v>702.45</v>
       </c>
@@ -3365,32 +4785,32 @@
       <c r="D24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="42"/>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42"/>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42"/>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
-      <c r="M24" s="42"/>
+      <c r="F24" s="46"/>
+      <c r="G24" s="46"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="46"/>
+      <c r="J24" s="46"/>
+      <c r="K24" s="46"/>
+      <c r="L24" s="46"/>
+      <c r="M24" s="46"/>
       <c r="N24" s="16">
         <v>-50</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="14.25" thickBot="1">
-      <c r="B25" s="43"/>
-      <c r="C25" s="44"/>
-      <c r="D25" s="44"/>
-      <c r="E25" s="44"/>
-      <c r="F25" s="44"/>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44"/>
-      <c r="I25" s="44"/>
-      <c r="J25" s="44"/>
-      <c r="K25" s="44"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="48"/>
+      <c r="D25" s="48"/>
+      <c r="E25" s="48"/>
+      <c r="F25" s="48"/>
+      <c r="G25" s="48"/>
+      <c r="H25" s="48"/>
+      <c r="I25" s="48"/>
+      <c r="J25" s="48"/>
+      <c r="K25" s="48"/>
       <c r="L25" s="2">
         <v>0</v>
       </c>
@@ -3402,30 +4822,35 @@
       </c>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="45" t="s">
+      <c r="B26" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="46"/>
-      <c r="D26" s="46"/>
-      <c r="E26" s="46"/>
-      <c r="F26" s="46" t="s">
+      <c r="C26" s="50"/>
+      <c r="D26" s="50"/>
+      <c r="E26" s="50"/>
+      <c r="F26" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="46"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="46"/>
-      <c r="K26" s="46" t="s">
-        <v>0</v>
-      </c>
-      <c r="L26" s="46"/>
-      <c r="M26" s="46">
+      <c r="G26" s="50"/>
+      <c r="H26" s="50"/>
+      <c r="I26" s="50"/>
+      <c r="J26" s="50"/>
+      <c r="K26" s="50" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="50"/>
+      <c r="M26" s="50">
         <v>745.39</v>
       </c>
-      <c r="N26" s="47"/>
+      <c r="N26" s="51"/>
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="E5:M5"/>
+    <mergeCell ref="E6:M6"/>
+    <mergeCell ref="E9:M9"/>
+    <mergeCell ref="E11:M11"/>
+    <mergeCell ref="E14:M14"/>
     <mergeCell ref="E16:M16"/>
     <mergeCell ref="E18:M18"/>
     <mergeCell ref="E24:M24"/>
@@ -3434,11 +4859,6 @@
     <mergeCell ref="F26:J26"/>
     <mergeCell ref="K26:L26"/>
     <mergeCell ref="M26:N26"/>
-    <mergeCell ref="E5:M5"/>
-    <mergeCell ref="E6:M6"/>
-    <mergeCell ref="E9:M9"/>
-    <mergeCell ref="E11:M11"/>
-    <mergeCell ref="E14:M14"/>
   </mergeCells>
   <phoneticPr fontId="9"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Hệ thống các ngành kinh tế vn
</commit_message>
<xml_diff>
--- a/Monthly Statement.xlsx
+++ b/Monthly Statement.xlsx
@@ -4,13 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue" sheetId="3" r:id="rId1"/>
     <sheet name="OPERATIONS" sheetId="4" r:id="rId2"/>
     <sheet name="June 2018" sheetId="5" r:id="rId3"/>
     <sheet name="May 2018" sheetId="2" r:id="rId4"/>
+    <sheet name="Q&amp;A" sheetId="7" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OPERATIONS!$B$3:$G$21</definedName>
@@ -104,7 +105,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="381" uniqueCount="225">
   <si>
     <t>Closed Trade P/L:</t>
   </si>
@@ -691,6 +692,130 @@
   </si>
   <si>
     <t>Pass</t>
+  </si>
+  <si>
+    <t>Thủ tục thành lập doanh nghiệp và phí bao nhiêu ?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://chamsocdoanhnghiep.com/bang-gia-dich-vu-tu-van-doanh-nghiep/</t>
+  </si>
+  <si>
+    <t>Doanh nghiệp tư nhân là gì ?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://www.ketoancattuong.vn/dich-vu/62/doanh-nghiep-tu-nhan-la-gi-.html</t>
+  </si>
+  <si>
+    <t>http://tuvanthanhlapcongtytnhh.com/tu-van-thanh-lap-cong-ty-tnhh/dac-diem-doanh-nghiep-tu-nhan-va-cong-ty-tnhh.html</t>
+  </si>
+  <si>
+    <t>Công ty trách nhiệm hữu hạn là gì ?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://vi.wikipedia.org/wiki/C%C3%B4ng_ty_tr%C3%A1ch_nhi%E1%BB%87m_h%E1%BB%AFu_h%E1%BA%A1n</t>
+  </si>
+  <si>
+    <t>Công ty cổ phần là gì?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://giayphepkinhdoanh.vn/cong-ty-co-phan-la-gi/</t>
+  </si>
+  <si>
+    <t>Chọn loại hình kinh doanh và đăng ký kinh doanh</t>
+  </si>
+  <si>
+    <t>http://business.gov.vn/tabid/100/catid/629/item/10907/ch%E1%BB%8Dn-lo%E1%BA%A1i-hinh-kinh-doanh-va-%C4%91%C4%83ng-ky-kinh-doanh.aspx</t>
+  </si>
+  <si>
+    <t>Công ty hợp danh là gì ?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://vi.wikipedia.org/wiki/C%C3%B4ng_ty_h%E1%BB%A3p_danh</t>
+  </si>
+  <si>
+    <t>Khái niệm thuế môn bài là gì?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://www.daotaoketoanhcm.com/thu-vien/phap-luat-thue/thue-mon-bai/khai-niem-thue-mon-bai-la-gi/</t>
+  </si>
+  <si>
+    <t>http://business.gov.vn/tabid/103/catid/638/item/11297/thu%E1%BA%BF-mon-bai.aspx</t>
+  </si>
+  <si>
+    <t>http://business.gov.vn/tabid/103/catid/638/item/11296/thu%E1%BA%BF-thu-nh%E1%BA%ADp-doanh-nghi%E1%BB%87p-va-thu%E1%BA%BF-thu-nh%E1%BA%ADp-h%E1%BB%99-gia-%C4%91inh.aspx</t>
+  </si>
+  <si>
+    <t>GỢI Ý TRONG VIỆC THÀNH LẬP CÔNG TY</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> HÀNH HỆ THỐNG NGÀNH KINH TẾ VIỆT NAM</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://dangkykinhdoanh.gov.vn/Default.aspx?tabid=106&amp;ArticleID=274&amp;language=en-GB</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://www.ketoancattuong.vn/trang/quy-trinh-thanh-lap-cong-ty.html</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <r>
+      <t>Thuế thu nhập doanh nghiệp và thuế thu nhập hộ gia đình </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF333333"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>  </t>
+    </r>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://ketoanthienung.org/tin-tuc/cac-khoan-thu-nhap-duoc-mien-thue-thu-nhap-doanh-nghiep.htm</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>Các khoản thu nhập được miễn thuế TNDN</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://ketoanthienung.org/tin-tuc/thue-suat-thue-thu-nhap-doanh-nghiep-nam-2014.htm</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://i-law.vn/blog/doanh-nghiep-132/kinh-doanh-thua-lo-doanh-nghiep-co-nop-thue-thu-nhap-doanh-nghiep-54069</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>http://business.gov.vn/tabid/110/catid/438/item/7029/gi%E1%BA%A5y-ph%C3%A9p-ho%E1%BA%A1t-%C4%91%E1%BB%99ng-ngo%E1%BA%A1i-h%E1%BB%91i-%C4%91%E1%BB%91i-v%E1%BB%9Bi-t%E1%BB%95-ch%E1%BB%A9c-t%C3%ADn-d%E1%BB%A5ng-phi-ng%C3%A2n-h%C3%A0ng.aspx</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>Giấy phép hoạt động ngoại hối đối với tổ chức tín dụng phi ngân hàng</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>Đầu tư bằng hình thức Forex rút tiền tại Việt Nam có phạm luật không ?</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://luatminhkhue.vn/tu-van-luat-doanh-nghiep/dau-tu-bang-hinh-thuc-forex-rut-tien-tai-viet-nam-co-pham-luat-khong-.aspx</t>
+    <phoneticPr fontId="8"/>
+  </si>
+  <si>
+    <t>https://luatminhgia.com.vn/hoi-dap-doanh-nghiep/-hoat-dong-kinh-doanh-ngoai-hoi-tai-viet-nam.aspx</t>
+    <phoneticPr fontId="8"/>
   </si>
 </sst>
 </file>
@@ -704,7 +829,7 @@
     <numFmt numFmtId="179" formatCode="[$$-409]#,##0.00_);[Red]\([$$-409]#,##0.00\)"/>
     <numFmt numFmtId="180" formatCode="#,##0.00&quot;%&quot;"/>
   </numFmts>
-  <fonts count="16">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -809,6 +934,13 @@
       <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF333333"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1641,10 +1773,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
@@ -4974,4 +5106,212 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:B44"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetData>
+    <row r="2" spans="1:2">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="B3" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="B6" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="B7" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>3</v>
+      </c>
+      <c r="B9" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="B10" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2">
+      <c r="A12">
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2">
+      <c r="B13" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2">
+      <c r="A15">
+        <v>5</v>
+      </c>
+      <c r="B15" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2">
+      <c r="B16" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2">
+      <c r="A18">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2">
+      <c r="B19" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2">
+      <c r="A21">
+        <v>7</v>
+      </c>
+      <c r="B21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2">
+      <c r="B22" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2">
+      <c r="B23" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" ht="15.75">
+      <c r="A25">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2">
+      <c r="B26" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2">
+      <c r="B27" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2">
+      <c r="A29">
+        <v>9</v>
+      </c>
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2">
+      <c r="B30" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2">
+      <c r="A32">
+        <v>10</v>
+      </c>
+      <c r="B32" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="B33" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35">
+        <v>11</v>
+      </c>
+      <c r="B35" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="B36" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="B37" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39">
+        <v>12</v>
+      </c>
+      <c r="B39" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="B40" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="B41" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43">
+        <v>13</v>
+      </c>
+      <c r="B43" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="B44" t="s">
+        <v>223</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update history of trade
</commit_message>
<xml_diff>
--- a/Monthly Statement.xlsx
+++ b/Monthly Statement.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11760" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue" sheetId="3" r:id="rId1"/>
-    <sheet name="OPERATIONS" sheetId="4" r:id="rId2"/>
-    <sheet name="June 2018" sheetId="5" r:id="rId3"/>
-    <sheet name="May 2018" sheetId="2" r:id="rId4"/>
-    <sheet name="Q&amp;A" sheetId="7" r:id="rId5"/>
+    <sheet name="History of Trading" sheetId="8" r:id="rId2"/>
+    <sheet name="OPERATIONS" sheetId="4" r:id="rId3"/>
+    <sheet name="June 2018" sheetId="5" r:id="rId4"/>
+    <sheet name="May 2018" sheetId="2" r:id="rId5"/>
+    <sheet name="Q&amp;A" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">OPERATIONS!$B$3:$G$21</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">OPERATIONS!$B$3:$G$21</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -105,7 +106,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="266">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="276">
   <si>
     <t>Closed Trade P/L:</t>
   </si>
@@ -991,23 +992,53 @@
     <t>https://www.chungkhoanviet.vn/tanman/13326</t>
     <phoneticPr fontId="8"/>
   </si>
+  <si>
+    <t>History of Trading</t>
+  </si>
+  <si>
+    <t>SELL</t>
+  </si>
+  <si>
+    <t>Session</t>
+  </si>
+  <si>
+    <t>Open Time</t>
+  </si>
+  <si>
+    <t>Close Time</t>
+  </si>
+  <si>
+    <t>Volume</t>
+  </si>
+  <si>
+    <t>Profit</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="5">
-    <numFmt numFmtId="176" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="177" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="178" formatCode="&quot;$&quot;#,##0.00"/>
-    <numFmt numFmtId="179" formatCode="[$$-409]#,##0.00_);[Red]\([$$-409]#,##0.00\)"/>
-    <numFmt numFmtId="180" formatCode="#,##0.00&quot;%&quot;"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00;[Red]\-&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
+    <numFmt numFmtId="165" formatCode="[$$-409]#,##0.00_);[Red]\([$$-409]#,##0.00\)"/>
+    <numFmt numFmtId="166" formatCode="#,##0.00&quot;%&quot;"/>
   </numFmts>
   <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1040,7 +1071,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1059,7 +1090,7 @@
     </font>
     <font>
       <sz val="6"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1120,7 +1151,7 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="游ゴシック"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -1177,7 +1208,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1397,14 +1428,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="177" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="91">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1472,14 +1516,14 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="180" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="9" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
@@ -1535,9 +1579,9 @@
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="17" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="180" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1546,10 +1590,10 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="179" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="178" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1559,8 +1603,8 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1572,6 +1616,7 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1617,7 +1662,20 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="19" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Currency" xfId="2" builtinId="4"/>
@@ -1989,20 +2047,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="K17" sqref="H17:K21"/>
+      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="10.375" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="10.42578125" style="18" customWidth="1"/>
     <col min="3" max="7" width="14" style="18" customWidth="1"/>
-    <col min="8" max="8" width="11.625" style="18" customWidth="1"/>
+    <col min="8" max="8" width="11.5703125" style="18" customWidth="1"/>
     <col min="9" max="9" width="14" style="18" customWidth="1"/>
-    <col min="10" max="16384" width="9.125" style="18"/>
+    <col min="10" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="15.75" customHeight="1">
@@ -2258,11 +2316,11 @@
         <v>90</v>
       </c>
       <c r="F10" s="57">
-        <v>1002.36</v>
+        <v>156.41999999999999</v>
       </c>
       <c r="G10" s="56">
         <f t="shared" si="0"/>
-        <v>6972.4199999999992</v>
+        <v>6126.48</v>
       </c>
       <c r="H10" s="56">
         <f t="shared" si="1"/>
@@ -2270,7 +2328,7 @@
       </c>
       <c r="I10" s="34">
         <f t="shared" si="2"/>
-        <v>18.025564103325713</v>
+        <v>4.0662963733032349</v>
       </c>
       <c r="J10" s="54" t="s">
         <v>190</v>
@@ -2302,13 +2360,13 @@
       </c>
       <c r="F12" s="62">
         <f>SUM(F4:F11)</f>
-        <v>2634.01</v>
+        <v>1788.0700000000002</v>
       </c>
       <c r="G12" s="60"/>
       <c r="H12" s="63"/>
       <c r="I12" s="58">
         <f>AVERAGE(I5:I11)</f>
-        <v>17.365147842573595</v>
+        <v>15.038603220903184</v>
       </c>
       <c r="J12" s="63"/>
     </row>
@@ -2456,39 +2514,249 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="2" max="8" width="10.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9">
+      <c r="B2" s="94" t="s">
+        <v>266</v>
+      </c>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
+      <c r="E2" s="95"/>
+      <c r="F2" s="95"/>
+      <c r="G2" s="95"/>
+      <c r="H2" s="95"/>
+      <c r="I2" s="96"/>
+    </row>
+    <row r="3" spans="2:9">
+      <c r="B3" s="93" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="93" t="s">
+        <v>274</v>
+      </c>
+      <c r="D3" s="93" t="s">
+        <v>271</v>
+      </c>
+      <c r="E3" s="93" t="s">
+        <v>268</v>
+      </c>
+      <c r="F3" s="93" t="s">
+        <v>269</v>
+      </c>
+      <c r="G3" s="93" t="s">
+        <v>270</v>
+      </c>
+      <c r="H3" s="93" t="s">
+        <v>272</v>
+      </c>
+      <c r="I3" s="93" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9">
+      <c r="B4" s="92" t="s">
+        <v>267</v>
+      </c>
+      <c r="C4" s="92"/>
+      <c r="D4" s="92"/>
+      <c r="E4" s="92" t="s">
+        <v>273</v>
+      </c>
+      <c r="F4" s="92"/>
+      <c r="G4" s="92"/>
+      <c r="H4" s="91"/>
+      <c r="I4" s="92"/>
+    </row>
+    <row r="5" spans="2:9">
+      <c r="B5" s="92"/>
+      <c r="C5" s="92"/>
+      <c r="D5" s="92"/>
+      <c r="E5" s="92"/>
+      <c r="F5" s="92"/>
+      <c r="G5" s="92"/>
+      <c r="H5" s="91"/>
+      <c r="I5" s="92"/>
+    </row>
+    <row r="6" spans="2:9">
+      <c r="B6" s="92"/>
+      <c r="C6" s="92"/>
+      <c r="D6" s="92"/>
+      <c r="E6" s="92"/>
+      <c r="F6" s="92"/>
+      <c r="G6" s="92"/>
+      <c r="H6" s="91"/>
+      <c r="I6" s="92"/>
+    </row>
+    <row r="7" spans="2:9">
+      <c r="B7" s="92"/>
+      <c r="C7" s="92"/>
+      <c r="D7" s="92"/>
+      <c r="E7" s="92"/>
+      <c r="F7" s="92"/>
+      <c r="G7" s="92"/>
+      <c r="H7" s="91"/>
+      <c r="I7" s="92"/>
+    </row>
+    <row r="8" spans="2:9">
+      <c r="B8" s="92"/>
+      <c r="C8" s="92"/>
+      <c r="D8" s="92"/>
+      <c r="E8" s="92"/>
+      <c r="F8" s="92"/>
+      <c r="G8" s="92"/>
+      <c r="H8" s="91"/>
+      <c r="I8" s="92"/>
+    </row>
+    <row r="9" spans="2:9">
+      <c r="B9" s="92"/>
+      <c r="C9" s="92"/>
+      <c r="D9" s="92"/>
+      <c r="E9" s="92"/>
+      <c r="F9" s="92"/>
+      <c r="G9" s="92"/>
+      <c r="H9" s="91"/>
+      <c r="I9" s="92"/>
+    </row>
+    <row r="10" spans="2:9">
+      <c r="B10" s="92"/>
+      <c r="C10" s="92"/>
+      <c r="D10" s="92"/>
+      <c r="E10" s="92"/>
+      <c r="F10" s="92"/>
+      <c r="G10" s="92"/>
+      <c r="H10" s="91"/>
+      <c r="I10" s="92"/>
+    </row>
+    <row r="11" spans="2:9">
+      <c r="B11" s="92"/>
+      <c r="C11" s="92"/>
+      <c r="D11" s="92"/>
+      <c r="E11" s="92"/>
+      <c r="F11" s="92"/>
+      <c r="G11" s="92"/>
+      <c r="H11" s="91"/>
+      <c r="I11" s="92"/>
+    </row>
+    <row r="12" spans="2:9">
+      <c r="B12" s="92"/>
+      <c r="C12" s="92"/>
+      <c r="D12" s="92"/>
+      <c r="E12" s="92"/>
+      <c r="F12" s="92"/>
+      <c r="G12" s="92"/>
+      <c r="H12" s="91"/>
+      <c r="I12" s="92"/>
+    </row>
+    <row r="13" spans="2:9">
+      <c r="B13" s="92"/>
+      <c r="C13" s="92"/>
+      <c r="D13" s="92"/>
+      <c r="E13" s="92"/>
+      <c r="F13" s="92"/>
+      <c r="G13" s="92"/>
+      <c r="H13" s="91"/>
+      <c r="I13" s="92"/>
+    </row>
+    <row r="14" spans="2:9">
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
+      <c r="H14" s="91"/>
+      <c r="I14" s="92"/>
+    </row>
+    <row r="15" spans="2:9">
+      <c r="B15" s="92"/>
+      <c r="C15" s="92"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="92"/>
+      <c r="F15" s="92"/>
+      <c r="G15" s="92"/>
+      <c r="H15" s="91"/>
+      <c r="I15" s="92"/>
+    </row>
+    <row r="16" spans="2:9">
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
+      <c r="E16" s="92"/>
+      <c r="F16" s="92"/>
+      <c r="G16" s="92"/>
+      <c r="H16" s="91"/>
+      <c r="I16" s="92"/>
+    </row>
+    <row r="17" spans="2:9">
+      <c r="B17" s="92"/>
+      <c r="C17" s="92"/>
+      <c r="D17" s="92"/>
+      <c r="E17" s="92"/>
+      <c r="F17" s="92"/>
+      <c r="G17" s="92"/>
+      <c r="H17" s="91"/>
+      <c r="I17" s="92"/>
+    </row>
+  </sheetData>
+  <dataConsolidate/>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B4:B17">
+      <formula1>"SELL,BUY"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E4:E17">
+      <formula1>"AM,PM"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr filterMode="1"/>
   <dimension ref="B1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9.125" style="18"/>
-    <col min="2" max="2" width="13.125" style="18" customWidth="1"/>
-    <col min="3" max="3" width="19.875" style="18" customWidth="1"/>
-    <col min="4" max="4" width="13.125" style="18" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="18"/>
+    <col min="2" max="2" width="13.140625" style="18" customWidth="1"/>
+    <col min="3" max="3" width="19.85546875" style="18" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="18" customWidth="1"/>
     <col min="5" max="5" width="17" style="18" customWidth="1"/>
-    <col min="6" max="7" width="13.125" style="18" customWidth="1"/>
-    <col min="8" max="16384" width="9.125" style="18"/>
+    <col min="6" max="7" width="13.140625" style="18" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:7">
-      <c r="B1" s="75" t="s">
+      <c r="B1" s="76" t="s">
         <v>103</v>
       </c>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
+      <c r="C1" s="76"/>
+      <c r="D1" s="76"/>
+      <c r="E1" s="76"/>
+      <c r="F1" s="76"/>
+      <c r="G1" s="76"/>
     </row>
     <row r="2" spans="2:7">
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
+      <c r="B2" s="76"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="24" t="s">
@@ -2873,13 +3141,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N40"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:14" s="1" customFormat="1" ht="23.25" thickBot="1">
       <c r="A1" s="64">
@@ -2925,7 +3193,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="2" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B2" s="47">
         <v>130907515</v>
       </c>
@@ -2935,22 +3203,22 @@
       <c r="D2" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="81" t="s">
+      <c r="E2" s="82" t="s">
         <v>111</v>
       </c>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="81"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="82"/>
       <c r="N2" s="48" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="3" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B3" s="49">
         <v>137714682</v>
       </c>
@@ -2991,7 +3259,7 @@
         <v>31.93</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="4" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B4" s="47">
         <v>137763688</v>
       </c>
@@ -3032,7 +3300,7 @@
         <v>36.47</v>
       </c>
     </row>
-    <row r="5" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="5" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B5" s="49">
         <v>138022429</v>
       </c>
@@ -3073,7 +3341,7 @@
         <v>6.25</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="6" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B6" s="47">
         <v>138393922</v>
       </c>
@@ -3114,7 +3382,7 @@
         <v>23.6</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="7" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B7" s="49">
         <v>138461980</v>
       </c>
@@ -3124,22 +3392,22 @@
       <c r="D7" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E7" s="82" t="s">
+      <c r="E7" s="83" t="s">
         <v>124</v>
       </c>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="82"/>
+      <c r="F7" s="83"/>
+      <c r="G7" s="83"/>
+      <c r="H7" s="83"/>
+      <c r="I7" s="83"/>
+      <c r="J7" s="83"/>
+      <c r="K7" s="83"/>
+      <c r="L7" s="83"/>
+      <c r="M7" s="83"/>
       <c r="N7" s="52">
         <v>-100</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="8" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B8" s="47">
         <v>138475841</v>
       </c>
@@ -3180,7 +3448,7 @@
         <v>48.47</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="9" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B9" s="49">
         <v>138654225</v>
       </c>
@@ -3221,7 +3489,7 @@
         <v>2.4900000000000002</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="10" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B10" s="47">
         <v>138723413</v>
       </c>
@@ -3231,22 +3499,22 @@
       <c r="D10" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E10" s="81" t="s">
+      <c r="E10" s="82" t="s">
         <v>131</v>
       </c>
-      <c r="F10" s="81"/>
-      <c r="G10" s="81"/>
-      <c r="H10" s="81"/>
-      <c r="I10" s="81"/>
-      <c r="J10" s="81"/>
-      <c r="K10" s="81"/>
-      <c r="L10" s="81"/>
-      <c r="M10" s="81"/>
+      <c r="F10" s="82"/>
+      <c r="G10" s="82"/>
+      <c r="H10" s="82"/>
+      <c r="I10" s="82"/>
+      <c r="J10" s="82"/>
+      <c r="K10" s="82"/>
+      <c r="L10" s="82"/>
+      <c r="M10" s="82"/>
       <c r="N10" s="48">
         <v>-20</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="11" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B11" s="49">
         <v>138732442</v>
       </c>
@@ -3287,7 +3555,7 @@
         <v>0.82</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="12" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B12" s="47">
         <v>138736541</v>
       </c>
@@ -3328,7 +3596,7 @@
         <v>11.35</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="13" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B13" s="49">
         <v>138897659</v>
       </c>
@@ -3369,7 +3637,7 @@
         <v>34.58</v>
       </c>
     </row>
-    <row r="14" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="14" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B14" s="47">
         <v>138953312</v>
       </c>
@@ -3410,7 +3678,7 @@
         <v>9.68</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="15" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B15" s="49">
         <v>138963274</v>
       </c>
@@ -3451,7 +3719,7 @@
         <v>32.78</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="16" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B16" s="47">
         <v>139069945</v>
       </c>
@@ -3492,7 +3760,7 @@
         <v>-31.59</v>
       </c>
     </row>
-    <row r="17" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="17" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B17" s="49">
         <v>139070001</v>
       </c>
@@ -3533,7 +3801,7 @@
         <v>-7.75</v>
       </c>
     </row>
-    <row r="18" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="18" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B18" s="47">
         <v>139076560</v>
       </c>
@@ -3574,7 +3842,7 @@
         <v>10.39</v>
       </c>
     </row>
-    <row r="19" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="19" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B19" s="49">
         <v>139121598</v>
       </c>
@@ -3615,7 +3883,7 @@
         <v>66.22</v>
       </c>
     </row>
-    <row r="20" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="20" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B20" s="47">
         <v>139177488</v>
       </c>
@@ -3656,7 +3924,7 @@
         <v>7.51</v>
       </c>
     </row>
-    <row r="21" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="21" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B21" s="49">
         <v>139189288</v>
       </c>
@@ -3697,7 +3965,7 @@
         <v>23.07</v>
       </c>
     </row>
-    <row r="22" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="22" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B22" s="47">
         <v>139193605</v>
       </c>
@@ -3738,7 +4006,7 @@
         <v>11.49</v>
       </c>
     </row>
-    <row r="23" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="23" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B23" s="49">
         <v>139209052</v>
       </c>
@@ -3779,7 +4047,7 @@
         <v>60.22</v>
       </c>
     </row>
-    <row r="24" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="24" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B24" s="47">
         <v>139249180</v>
       </c>
@@ -3789,22 +4057,22 @@
       <c r="D24" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="81" t="s">
+      <c r="E24" s="82" t="s">
         <v>161</v>
       </c>
-      <c r="F24" s="81"/>
-      <c r="G24" s="81"/>
-      <c r="H24" s="81"/>
-      <c r="I24" s="81"/>
-      <c r="J24" s="81"/>
-      <c r="K24" s="81"/>
-      <c r="L24" s="81"/>
-      <c r="M24" s="81"/>
+      <c r="F24" s="82"/>
+      <c r="G24" s="82"/>
+      <c r="H24" s="82"/>
+      <c r="I24" s="82"/>
+      <c r="J24" s="82"/>
+      <c r="K24" s="82"/>
+      <c r="L24" s="82"/>
+      <c r="M24" s="82"/>
       <c r="N24" s="48">
         <v>699.54</v>
       </c>
     </row>
-    <row r="25" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="25" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B25" s="49">
         <v>139254304</v>
       </c>
@@ -3845,7 +4113,7 @@
         <v>58.1</v>
       </c>
     </row>
-    <row r="26" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="26" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B26" s="47">
         <v>139288612</v>
       </c>
@@ -3886,7 +4154,7 @@
         <v>31.29</v>
       </c>
     </row>
-    <row r="27" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="27" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B27" s="49">
         <v>139320132</v>
       </c>
@@ -3927,7 +4195,7 @@
         <v>10.23</v>
       </c>
     </row>
-    <row r="28" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="28" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B28" s="47">
         <v>139321846</v>
       </c>
@@ -3968,7 +4236,7 @@
         <v>126.17</v>
       </c>
     </row>
-    <row r="29" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="29" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B29" s="49">
         <v>139344009</v>
       </c>
@@ -4009,7 +4277,7 @@
         <v>2.48</v>
       </c>
     </row>
-    <row r="30" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="30" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B30" s="47">
         <v>139373451</v>
       </c>
@@ -4050,7 +4318,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="31" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="31" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B31" s="49">
         <v>139381854</v>
       </c>
@@ -4091,7 +4359,7 @@
         <v>4.58</v>
       </c>
     </row>
-    <row r="32" spans="2:14" s="1" customFormat="1" thickBot="1">
+    <row r="32" spans="2:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B32" s="47">
         <v>139407314</v>
       </c>
@@ -4132,7 +4400,7 @@
         <v>-26.91</v>
       </c>
     </row>
-    <row r="33" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="33" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B33" s="49">
         <v>139426625</v>
       </c>
@@ -4173,7 +4441,7 @@
         <v>120.79</v>
       </c>
     </row>
-    <row r="34" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="34" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B34" s="47">
         <v>139619569</v>
       </c>
@@ -4214,7 +4482,7 @@
         <v>-1.92</v>
       </c>
     </row>
-    <row r="35" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="35" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B35" s="49">
         <v>139619621</v>
       </c>
@@ -4255,7 +4523,7 @@
         <v>7.2</v>
       </c>
     </row>
-    <row r="36" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="36" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B36" s="47">
         <v>139682129</v>
       </c>
@@ -4296,7 +4564,7 @@
         <v>27.01</v>
       </c>
     </row>
-    <row r="37" spans="1:14" s="1" customFormat="1" thickBot="1">
+    <row r="37" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
       <c r="B37" s="49">
         <v>139780262</v>
       </c>
@@ -4306,32 +4574,32 @@
       <c r="D37" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="E37" s="82" t="s">
+      <c r="E37" s="83" t="s">
         <v>187</v>
       </c>
-      <c r="F37" s="82"/>
-      <c r="G37" s="82"/>
-      <c r="H37" s="82"/>
-      <c r="I37" s="82"/>
-      <c r="J37" s="82"/>
-      <c r="K37" s="82"/>
-      <c r="L37" s="82"/>
-      <c r="M37" s="82"/>
+      <c r="F37" s="83"/>
+      <c r="G37" s="83"/>
+      <c r="H37" s="83"/>
+      <c r="I37" s="83"/>
+      <c r="J37" s="83"/>
+      <c r="K37" s="83"/>
+      <c r="L37" s="83"/>
+      <c r="M37" s="83"/>
       <c r="N37" s="52">
         <v>-150</v>
       </c>
     </row>
-    <row r="38" spans="1:14" s="1" customFormat="1" thickBot="1">
-      <c r="B38" s="76"/>
-      <c r="C38" s="77"/>
-      <c r="D38" s="77"/>
-      <c r="E38" s="77"/>
-      <c r="F38" s="77"/>
-      <c r="G38" s="77"/>
-      <c r="H38" s="77"/>
-      <c r="I38" s="77"/>
-      <c r="J38" s="77"/>
-      <c r="K38" s="77"/>
+    <row r="38" spans="1:14" s="1" customFormat="1" ht="14.25" thickBot="1">
+      <c r="B38" s="77"/>
+      <c r="C38" s="78"/>
+      <c r="D38" s="78"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="78"/>
+      <c r="G38" s="78"/>
+      <c r="H38" s="78"/>
+      <c r="I38" s="78"/>
+      <c r="J38" s="78"/>
+      <c r="K38" s="78"/>
       <c r="L38" s="43">
         <v>0</v>
       </c>
@@ -4343,27 +4611,27 @@
       </c>
     </row>
     <row r="39" spans="1:14" s="1" customFormat="1" ht="13.5">
-      <c r="B39" s="78" t="s">
+      <c r="B39" s="79" t="s">
         <v>188</v>
       </c>
-      <c r="C39" s="79"/>
-      <c r="D39" s="79"/>
-      <c r="E39" s="79"/>
-      <c r="F39" s="79" t="s">
+      <c r="C39" s="80"/>
+      <c r="D39" s="80"/>
+      <c r="E39" s="80"/>
+      <c r="F39" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="G39" s="79"/>
-      <c r="H39" s="79"/>
-      <c r="I39" s="79"/>
-      <c r="J39" s="79"/>
-      <c r="K39" s="79" t="s">
-        <v>0</v>
-      </c>
-      <c r="L39" s="79"/>
-      <c r="M39" s="79">
+      <c r="G39" s="80"/>
+      <c r="H39" s="80"/>
+      <c r="I39" s="80"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80" t="s">
+        <v>0</v>
+      </c>
+      <c r="L39" s="80"/>
+      <c r="M39" s="80">
         <v>726.18</v>
       </c>
-      <c r="N39" s="80"/>
+      <c r="N39" s="81"/>
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
@@ -4388,15 +4656,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N26"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.125" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="13.5"/>
   <cols>
-    <col min="1" max="16384" width="9.125" style="1"/>
+    <col min="1" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="22.5">
@@ -4576,17 +4844,17 @@
       <c r="D5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E5" s="83" t="s">
+      <c r="E5" s="84" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="83"/>
-      <c r="G5" s="83"/>
-      <c r="H5" s="83"/>
-      <c r="I5" s="83"/>
-      <c r="J5" s="83"/>
-      <c r="K5" s="83"/>
-      <c r="L5" s="83"/>
-      <c r="M5" s="83"/>
+      <c r="F5" s="84"/>
+      <c r="G5" s="84"/>
+      <c r="H5" s="84"/>
+      <c r="I5" s="84"/>
+      <c r="J5" s="84"/>
+      <c r="K5" s="84"/>
+      <c r="L5" s="84"/>
+      <c r="M5" s="84"/>
       <c r="N5" s="15">
         <v>-100</v>
       </c>
@@ -4601,17 +4869,17 @@
       <c r="D6" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="85" t="s">
         <v>47</v>
       </c>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="84"/>
+      <c r="F6" s="85"/>
+      <c r="G6" s="85"/>
+      <c r="H6" s="85"/>
+      <c r="I6" s="85"/>
+      <c r="J6" s="85"/>
+      <c r="K6" s="85"/>
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
       <c r="N6" s="16">
         <v>100</v>
       </c>
@@ -4708,17 +4976,17 @@
       <c r="D9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="83" t="s">
+      <c r="E9" s="84" t="s">
         <v>40</v>
       </c>
-      <c r="F9" s="83"/>
-      <c r="G9" s="83"/>
-      <c r="H9" s="83"/>
-      <c r="I9" s="83"/>
-      <c r="J9" s="83"/>
-      <c r="K9" s="83"/>
-      <c r="L9" s="83"/>
-      <c r="M9" s="83"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="84"/>
+      <c r="K9" s="84"/>
+      <c r="L9" s="84"/>
+      <c r="M9" s="84"/>
       <c r="N9" s="15">
         <v>15.36</v>
       </c>
@@ -4774,17 +5042,17 @@
       <c r="D11" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="E11" s="83" t="s">
+      <c r="E11" s="84" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="83"/>
-      <c r="G11" s="83"/>
-      <c r="H11" s="83"/>
-      <c r="I11" s="83"/>
-      <c r="J11" s="83"/>
-      <c r="K11" s="83"/>
-      <c r="L11" s="83"/>
-      <c r="M11" s="83"/>
+      <c r="F11" s="84"/>
+      <c r="G11" s="84"/>
+      <c r="H11" s="84"/>
+      <c r="I11" s="84"/>
+      <c r="J11" s="84"/>
+      <c r="K11" s="84"/>
+      <c r="L11" s="84"/>
+      <c r="M11" s="84"/>
       <c r="N11" s="15">
         <v>-20</v>
       </c>
@@ -4881,17 +5149,17 @@
       <c r="D14" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E14" s="84" t="s">
+      <c r="E14" s="85" t="s">
         <v>28</v>
       </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="84"/>
+      <c r="F14" s="85"/>
+      <c r="G14" s="85"/>
+      <c r="H14" s="85"/>
+      <c r="I14" s="85"/>
+      <c r="J14" s="85"/>
+      <c r="K14" s="85"/>
+      <c r="L14" s="85"/>
+      <c r="M14" s="85"/>
       <c r="N14" s="16">
         <v>-50</v>
       </c>
@@ -4947,17 +5215,17 @@
       <c r="D16" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E16" s="84" t="s">
+      <c r="E16" s="85" t="s">
         <v>24</v>
       </c>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="84"/>
+      <c r="F16" s="85"/>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="85"/>
+      <c r="K16" s="85"/>
+      <c r="L16" s="85"/>
+      <c r="M16" s="85"/>
       <c r="N16" s="16">
         <v>-50</v>
       </c>
@@ -5013,17 +5281,17 @@
       <c r="D18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E18" s="84" t="s">
+      <c r="E18" s="85" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="84"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
+      <c r="L18" s="85"/>
+      <c r="M18" s="85"/>
       <c r="N18" s="16">
         <v>702.45</v>
       </c>
@@ -5243,32 +5511,32 @@
       <c r="D24" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E24" s="84" t="s">
+      <c r="E24" s="85" t="s">
         <v>3</v>
       </c>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
-      <c r="K24" s="84"/>
-      <c r="L24" s="84"/>
-      <c r="M24" s="84"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
+      <c r="L24" s="85"/>
+      <c r="M24" s="85"/>
       <c r="N24" s="16">
         <v>-50</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="14.25" thickBot="1">
-      <c r="B25" s="85"/>
-      <c r="C25" s="86"/>
-      <c r="D25" s="86"/>
-      <c r="E25" s="86"/>
-      <c r="F25" s="86"/>
-      <c r="G25" s="86"/>
-      <c r="H25" s="86"/>
-      <c r="I25" s="86"/>
-      <c r="J25" s="86"/>
-      <c r="K25" s="86"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="87"/>
+      <c r="D25" s="87"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="87"/>
+      <c r="I25" s="87"/>
+      <c r="J25" s="87"/>
+      <c r="K25" s="87"/>
       <c r="L25" s="2">
         <v>0</v>
       </c>
@@ -5280,27 +5548,27 @@
       </c>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="87" t="s">
+      <c r="B26" s="88" t="s">
         <v>2</v>
       </c>
-      <c r="C26" s="88"/>
-      <c r="D26" s="88"/>
-      <c r="E26" s="88"/>
-      <c r="F26" s="88" t="s">
+      <c r="C26" s="89"/>
+      <c r="D26" s="89"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="89" t="s">
         <v>1</v>
       </c>
-      <c r="G26" s="88"/>
-      <c r="H26" s="88"/>
-      <c r="I26" s="88"/>
-      <c r="J26" s="88"/>
-      <c r="K26" s="88" t="s">
-        <v>0</v>
-      </c>
-      <c r="L26" s="88"/>
-      <c r="M26" s="88">
+      <c r="G26" s="89"/>
+      <c r="H26" s="89"/>
+      <c r="I26" s="89"/>
+      <c r="J26" s="89"/>
+      <c r="K26" s="89" t="s">
+        <v>0</v>
+      </c>
+      <c r="L26" s="89"/>
+      <c r="M26" s="89">
         <v>745.39</v>
       </c>
-      <c r="N26" s="89"/>
+      <c r="N26" s="90"/>
     </row>
   </sheetData>
   <mergeCells count="13">
@@ -5324,15 +5592,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:C95"/>
   <sheetViews>
-    <sheetView topLeftCell="A67" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
       <selection activeCell="F97" sqref="F97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="16384" width="9" style="18"/>
   </cols>
@@ -5716,7 +5984,7 @@
       </c>
     </row>
     <row r="85" spans="1:3">
-      <c r="C85" s="90" t="s">
+      <c r="C85" s="75" t="s">
         <v>261</v>
       </c>
     </row>
@@ -5726,7 +5994,7 @@
       </c>
     </row>
     <row r="87" spans="1:3">
-      <c r="C87" s="90" t="s">
+      <c r="C87" s="75" t="s">
         <v>263</v>
       </c>
     </row>
@@ -5736,7 +6004,7 @@
       </c>
     </row>
     <row r="89" spans="1:3">
-      <c r="C89" s="90" t="s">
+      <c r="C89" s="75" t="s">
         <v>265</v>
       </c>
     </row>

</xml_diff>